<commit_message>
New csv for Tom
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dutch\Documents\WashU Data Bootcamp\07-Project-1\Project_1_Group_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A058D6D-590F-452B-BBB3-04368AB954C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF692E2-4492-4151-98FE-3613246AFC55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A796E1C-0AA8-422A-9BD3-9FCE38BDDCE2}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>St. Louis and St. Louis County</t>
   </si>
   <si>
-    <t>All businesses have a $, $$, $$$ or $$$$</t>
-  </si>
-  <si>
     <t>File</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>Note: choose same number of reviews as min(men vs women)</t>
+  </si>
+  <si>
+    <t>All businesses have a $, $$, $$$ or $$$$, after dropping duplicates</t>
   </si>
 </sst>
 </file>
@@ -716,7 +716,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -737,10 +737,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -751,85 +751,85 @@
         <v>477</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>1048</v>
+        <v>1419</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>62074</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>734</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="C19">
         <v>396</v>
@@ -837,7 +837,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>338</v>
@@ -851,10 +851,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23">
         <v>106</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24">
         <v>212</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25">
         <v>19</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -892,10 +892,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29">
         <v>151</v>
@@ -903,7 +903,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30">
         <v>227</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31">
         <v>17</v>
@@ -919,7 +919,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -933,27 +933,27 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" t="s">
         <v>27</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>28</v>
-      </c>
-      <c r="E35" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37">
         <v>18</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38">
         <v>62</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C39">
         <v>141</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40">
         <v>103</v>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41">
         <v>14</v>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran statistics for NYC, SEA, STL
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dutch\Documents\WashU Data Bootcamp\07-Project-1\Project_1_Group_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF692E2-4492-4151-98FE-3613246AFC55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5A42B3-B88A-42B2-93CE-EF3BFCDFD913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A796E1C-0AA8-422A-9BD3-9FCE38BDDCE2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Total ZIP Codes</t>
   </si>
@@ -111,31 +111,7 @@
     <t>Men vs Women Rating</t>
   </si>
   <si>
-    <t>men</t>
-  </si>
-  <si>
-    <t>women</t>
-  </si>
-  <si>
     <t>total</t>
-  </si>
-  <si>
-    <t>Bracket</t>
-  </si>
-  <si>
-    <t>0-3</t>
-  </si>
-  <si>
-    <t>3.0-3.5</t>
-  </si>
-  <si>
-    <t>3.5-4</t>
-  </si>
-  <si>
-    <t>4.0-4.5</t>
-  </si>
-  <si>
-    <t>4.5-5</t>
   </si>
   <si>
     <t>Note: choose same number of reviews as min(men vs women)</t>
@@ -215,16 +191,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>27660</xdr:rowOff>
+      <xdr:rowOff>35280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>288252</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>311112</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>60969</xdr:rowOff>
+      <xdr:rowOff>68589</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -253,7 +229,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9448800" y="2770860"/>
+          <a:off x="10690860" y="2778480"/>
           <a:ext cx="3214332" cy="2410749"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -265,16 +241,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>500520</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>439560</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>48120</xdr:rowOff>
+      <xdr:rowOff>2400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>57252</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>605892</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>81429</xdr:rowOff>
+      <xdr:rowOff>35709</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -303,7 +279,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6169800" y="2791320"/>
+          <a:off x="7328040" y="2745600"/>
           <a:ext cx="3214332" cy="2410749"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -315,16 +291,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>193320</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>139980</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>359652</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>306312</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>101889</xdr:rowOff>
+      <xdr:rowOff>86649</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -353,7 +329,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2814600" y="2811780"/>
+          <a:off x="3980460" y="2796540"/>
           <a:ext cx="3214332" cy="2410749"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -366,22 +342,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
+      <xdr:colOff>121920</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>45721</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>93345</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>102871</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{703B6AFA-83A2-497B-9B18-C5E03B4FAF42}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07E03913-69D3-47D2-84DD-8B9D2BC35ED8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -403,8 +379,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4061460" y="5425440"/>
-          <a:ext cx="3375660" cy="2531745"/>
+          <a:off x="3962400" y="5349241"/>
+          <a:ext cx="3733800" cy="2800350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -715,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B1878B9-24FD-4DB3-9524-C3338102EAE8}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,7 +727,7 @@
         <v>477</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -819,12 +795,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -835,7 +811,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
@@ -843,13 +819,13 @@
         <v>338</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C21">
         <f>SUM(C19:C20)</f>
         <v>734</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -859,38 +835,62 @@
       <c r="C23">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <f>C23*1</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C24">
         <v>212</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <f>C24*2</f>
+        <v>424</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C25">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <f>C25*3</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <f>C26*4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C27">
         <f>SUM(C23:C26)</f>
         <v>338</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <f>SUM(D23:D26)</f>
+        <v>591</v>
+      </c>
+      <c r="E27">
+        <f>D27/C27</f>
+        <v>1.7485207100591715</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -900,29 +900,45 @@
       <c r="C29">
         <v>151</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <f>C29*1</f>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C30">
         <v>227</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <f>C30*2</f>
+        <v>454</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C31">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <f>C31*3</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C32">
         <v>1</v>
+      </c>
+      <c r="D32">
+        <f>C32*4</f>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -930,6 +946,14 @@
         <f>SUM(C29:C32)</f>
         <v>396</v>
       </c>
+      <c r="D33">
+        <f>SUM(D29:D32)</f>
+        <v>660</v>
+      </c>
+      <c r="E33">
+        <f>D33/C33</f>
+        <v>1.6666666666666667</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
@@ -937,107 +961,104 @@
       </c>
       <c r="B35" s="1"/>
       <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" t="s">
         <v>26</v>
       </c>
-      <c r="D35" t="s">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36">
         <v>27</v>
       </c>
-      <c r="E35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="1" t="s">
-        <v>29</v>
+      <c r="D36">
+        <v>36</v>
+      </c>
+      <c r="E36">
+        <f>D36+C36</f>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="1" t="s">
-        <v>30</v>
+      <c r="B37" s="1">
+        <v>2</v>
       </c>
       <c r="C37">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D37">
         <v>17</v>
       </c>
       <c r="E37">
-        <v>38</v>
+        <f t="shared" ref="E37:E40" si="0">D37+C37</f>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="1" t="s">
-        <v>31</v>
+      <c r="B38" s="1">
+        <v>3</v>
       </c>
       <c r="C38">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D38">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="E38">
-        <v>132</v>
+        <f t="shared" si="0"/>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="1" t="s">
-        <v>32</v>
+      <c r="B39" s="1">
+        <v>4</v>
       </c>
       <c r="C39">
-        <v>141</v>
+        <v>97</v>
       </c>
       <c r="D39">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="E39">
-        <v>288</v>
+        <f t="shared" si="0"/>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="1" t="s">
-        <v>33</v>
+      <c r="B40" s="1">
+        <v>5</v>
       </c>
       <c r="C40">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="D40">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="E40">
-        <v>244</v>
+        <f t="shared" si="0"/>
+        <v>341</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B41" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="B41" s="1"/>
       <c r="C41">
-        <v>14</v>
+        <f>SUM(C36:C40)</f>
+        <v>338</v>
       </c>
       <c r="D41">
-        <v>17</v>
-      </c>
-      <c r="E41">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C42">
-        <f>SUM(C37:C41)</f>
+        <f>SUM(D36:D40)</f>
         <v>338</v>
-      </c>
-      <c r="D42">
-        <f>SUM(D37:D41)</f>
-        <v>338</v>
-      </c>
-      <c r="E42">
-        <f>SUM(E37:E41)</f>
-        <v>734</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>